<commit_message>
Smooth putter adjustement. Usart communication improved.
Quick fixes.
</commit_message>
<xml_diff>
--- a/model/GOLF/parameters.xlsx
+++ b/model/GOLF/parameters.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="405" windowWidth="14805" windowHeight="7710"/>
@@ -131,7 +131,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,7 +166,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>